<commit_message>
HW: Cost estimation updated
</commit_message>
<xml_diff>
--- a/hw/Cost Estimation.xlsx
+++ b/hw/Cost Estimation.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Daniel\ele\bat_source\hw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B54BF9-1F7B-494C-8C8D-E1EBD032DDBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2CCC01-424C-4536-B7C3-C66C683DBAC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" tabRatio="735" activeTab="4" xr2:uid="{23E9BD06-C4F9-4485-BC66-1FB5ADDDACFE}"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="17325" tabRatio="735" firstSheet="1" activeTab="6" xr2:uid="{23E9BD06-C4F9-4485-BC66-1FB5ADDDACFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Bestellungen Prototypen" sheetId="3" r:id="rId1"/>
-    <sheet name="Kostenübersicht Prototypen" sheetId="4" r:id="rId2"/>
+    <sheet name="Prototyp 1" sheetId="4" r:id="rId2"/>
     <sheet name="Fehlende Komponenten" sheetId="5" r:id="rId3"/>
     <sheet name="Zusatzkosten Verbesserung V2" sheetId="1" r:id="rId4"/>
     <sheet name="Kostenabschätzung" sheetId="6" r:id="rId5"/>
     <sheet name="Kostenabschätzung Serie Detail" sheetId="2" r:id="rId6"/>
+    <sheet name="Kostenabschätzung Serie Det (2)" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="360">
   <si>
     <t>LCD</t>
   </si>
@@ -4870,7 +4871,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5165,8 +5166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16E66A6-478A-46D0-9411-658E50B8984D}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5189,7 +5190,7 @@
         <v>342</v>
       </c>
       <c r="B5">
-        <f>'Kostenübersicht Prototypen'!B8</f>
+        <f>'Prototyp 1'!B8</f>
         <v>999.29</v>
       </c>
     </row>
@@ -5271,7 +5272,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5977,4 +5978,717 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AAF1535-E1EC-4FF6-AC48-63822CFED5D4}">
+  <dimension ref="A1:O25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="48.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="24" x14ac:dyDescent="0.4">
+      <c r="A1" s="32" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <f>SUM(C5:C1048576)</f>
+        <v>859.2299999999999</v>
+      </c>
+      <c r="D3">
+        <f>SUM(D5:D1048576)</f>
+        <v>2946.32</v>
+      </c>
+      <c r="E3">
+        <f>SUM(E5:E1048576)</f>
+        <v>3540.82</v>
+      </c>
+      <c r="G3">
+        <f>SUM(G5:G1048576)</f>
+        <v>171.84599999999998</v>
+      </c>
+      <c r="H3">
+        <f>SUM(H5:H1048576)</f>
+        <v>117.8528</v>
+      </c>
+      <c r="I3">
+        <f>SUM(I5:I1048576)</f>
+        <v>141.63279999999997</v>
+      </c>
+      <c r="M3">
+        <f>G3+M4</f>
+        <v>192.58599999999998</v>
+      </c>
+      <c r="N3">
+        <f>'Bestellungen Prototypen'!M1-'Kostenabschätzung Serie Det (2)'!M3</f>
+        <v>7.2720000000000198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4">
+        <f>SUM(L5:L21)</f>
+        <v>248.48000000000002</v>
+      </c>
+      <c r="M4">
+        <f>SUM(M5:M21)</f>
+        <v>20.74</v>
+      </c>
+      <c r="O4">
+        <f>I3+M4+N3+'Zusatzkosten Verbesserung V2'!B10</f>
+        <v>182.2448</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>30.4</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E6" si="0">C5/C$4*D$4</f>
+        <v>152</v>
+      </c>
+      <c r="G5">
+        <f>C5/C$4</f>
+        <v>6.08</v>
+      </c>
+      <c r="H5">
+        <f>D5/D$4</f>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f>E5/D$4</f>
+        <v>6.08</v>
+      </c>
+      <c r="K5" t="s">
+        <v>322</v>
+      </c>
+      <c r="L5">
+        <v>12.9</v>
+      </c>
+      <c r="M5">
+        <f>L5/5</f>
+        <v>2.58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <f>8+9.24+1.5</f>
+        <v>18.740000000000002</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>93.7</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:H25" si="1">C6/C$4</f>
+        <v>3.7480000000000002</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I25" si="2">E6/D$4</f>
+        <v>3.7480000000000002</v>
+      </c>
+      <c r="K6" t="s">
+        <v>323</v>
+      </c>
+      <c r="L6">
+        <v>60</v>
+      </c>
+      <c r="M6">
+        <f>L6/5</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>314</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>117</v>
+      </c>
+      <c r="E7">
+        <v>117</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>23.4</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>4.68</v>
+      </c>
+      <c r="K7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7">
+        <v>22.08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>507.35</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2290.94</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2290.94</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>101.47</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>91.637600000000006</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>91.637600000000006</v>
+      </c>
+      <c r="K8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="E9">
+        <f>C9/C$4*D$4</f>
+        <v>46</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>1.8399999999999999</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>1.84</v>
+      </c>
+      <c r="K9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9">
+        <f>10*1.38</f>
+        <v>13.799999999999999</v>
+      </c>
+      <c r="M9">
+        <f>L9/5</f>
+        <v>2.76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ref="E10:E16" si="3">C10/C$4*D$4</f>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L10">
+        <f>10*1.7</f>
+        <v>17</v>
+      </c>
+      <c r="M10">
+        <f>L10/5</f>
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>3.68</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>18.399999999999999</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="K11" t="s">
+        <v>313</v>
+      </c>
+      <c r="L11">
+        <v>44.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <f>3*5*0.2</f>
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <f>5*0.16</f>
+        <v>0.8</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0.16</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0.25</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="3"/>
+        <v>1.25</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <f>8*0.03</f>
+        <v>0.24</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>10.1</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>50.5</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>2.02</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>2.02</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2">
+        <v>139.38</v>
+      </c>
+      <c r="D18" s="2">
+        <v>655.38</v>
+      </c>
+      <c r="E18" s="2">
+        <v>655.38</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>27.875999999999998</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>26.215199999999999</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>26.215199999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1.03</v>
+      </c>
+      <c r="E19">
+        <f>C19/C$4*D$4</f>
+        <v>5.15</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>0.20600000000000002</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>0.20600000000000002</v>
+      </c>
+      <c r="K19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ref="E20:E25" si="4">C20/C$4*D$4</f>
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>5.8</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="4"/>
+        <v>28.999999999999996</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>1.2</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="2"/>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>6.5</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="4"/>
+        <v>32.5</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>1.3</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="2"/>
+        <v>1.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>